<commit_message>
Added tab to Excel
</commit_message>
<xml_diff>
--- a/SharpGP/Sharp_HowToGP.xlsx
+++ b/SharpGP/Sharp_HowToGP.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg0316779\Documents\Studia\ProgramowanieGenetyczne\SharpGP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\Documents\GitHub\ProgramowanieGenetyczne\SharpGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7679B6-D15E-4C05-BBDD-6B1E52126393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D1487F-59FE-4B0D-A952-44BD39A4C3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="3915" windowWidth="21600" windowHeight="12735" xr2:uid="{707DFE33-8F90-4A69-BDB2-B8E58753720D}"/>
+    <workbookView xWindow="495" yWindow="1350" windowWidth="16650" windowHeight="11295" activeTab="1" xr2:uid="{707DFE33-8F90-4A69-BDB2-B8E58753720D}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>What</t>
   </si>
@@ -145,6 +146,66 @@
   </si>
   <si>
     <t>swapActions/dropFunc</t>
+  </si>
+  <si>
+    <t>p1depth</t>
+  </si>
+  <si>
+    <t>n+</t>
+  </si>
+  <si>
+    <t>n-</t>
+  </si>
+  <si>
+    <t>mean-</t>
+  </si>
+  <si>
+    <t>mean+</t>
+  </si>
+  <si>
+    <t>(1+mean+ /mean- )</t>
+  </si>
+  <si>
+    <t>(1+mean- /mean+ )</t>
+  </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>1-p0</t>
+  </si>
+  <si>
+    <t>p+</t>
+  </si>
+  <si>
+    <t>p-</t>
+  </si>
+  <si>
+    <t>Suma p0,p+,p-</t>
+  </si>
+  <si>
+    <t>Program:</t>
+  </si>
+  <si>
+    <t>1 -&gt; 31 (16*1 + 15*'+')</t>
+  </si>
+  <si>
+    <t>2 -&gt; 8</t>
+  </si>
+  <si>
+    <t>3 -&gt; 4</t>
+  </si>
+  <si>
+    <t>4 -&gt; 2</t>
+  </si>
+  <si>
+    <t>5 -&gt; 1</t>
+  </si>
+  <si>
+    <t>6 -&gt; write( *5* )</t>
+  </si>
+  <si>
+    <t>7 -&gt; program</t>
   </si>
 </sst>
 </file>
@@ -187,7 +248,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -203,9 +264,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -243,7 +304,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -349,7 +410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -501,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED00169-7238-479B-899A-523C738036DD}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -747,4 +808,144 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C8AD3F-DE3B-4B12-A72F-BB3AA078B976}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>2+4+8+31</f>
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <f xml:space="preserve"> (1*31+2*8+3*4+4*2)/C2</f>
+        <v>1.4888888888888889</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <f>(1+E2/D2)</f>
+        <v>5.0298507462686564</v>
+      </c>
+      <c r="G2">
+        <f>(1+D2/E2)</f>
+        <v>1.2481481481481482</v>
+      </c>
+      <c r="I2">
+        <f>1/A2</f>
+        <v>0.2</v>
+      </c>
+      <c r="J2">
+        <f>1-I2</f>
+        <v>0.8</v>
+      </c>
+      <c r="K2">
+        <f>J2/(B2*F2)</f>
+        <v>0.15905044510385757</v>
+      </c>
+      <c r="L2">
+        <f>J2/G2</f>
+        <v>0.64094955489614247</v>
+      </c>
+      <c r="M2">
+        <f>I2+K2+L2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dodano arkusz weryfikujący prawdopodobieństwo
</commit_message>
<xml_diff>
--- a/SharpGP/Sharp_HowToGP.xlsx
+++ b/SharpGP/Sharp_HowToGP.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\Documents\GitHub\ProgramowanieGenetyczne\SharpGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D1487F-59FE-4B0D-A952-44BD39A4C3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DADC45-FD74-4C0B-8F62-F6489C58B39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="1350" windowWidth="16650" windowHeight="11295" activeTab="1" xr2:uid="{707DFE33-8F90-4A69-BDB2-B8E58753720D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{707DFE33-8F90-4A69-BDB2-B8E58753720D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
+    <sheet name="Grow And Mutate" sheetId="1" r:id="rId1"/>
+    <sheet name="Ruletka" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>What</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Grow</t>
   </si>
   <si>
-    <t>Mutation</t>
-  </si>
-  <si>
     <t>Program</t>
   </si>
   <si>
@@ -187,31 +184,49 @@
     <t>Program:</t>
   </si>
   <si>
-    <t>1 -&gt; 31 (16*1 + 15*'+')</t>
-  </si>
-  <si>
-    <t>2 -&gt; 8</t>
-  </si>
-  <si>
-    <t>3 -&gt; 4</t>
-  </si>
-  <si>
-    <t>4 -&gt; 2</t>
-  </si>
-  <si>
-    <t>5 -&gt; 1</t>
-  </si>
-  <si>
-    <t>6 -&gt; write( *5* )</t>
-  </si>
-  <si>
-    <t>7 -&gt; program</t>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>nodes</t>
+  </si>
+  <si>
+    <t>1*program</t>
+  </si>
+  <si>
+    <t>31 (16*'1' + 15*'+')</t>
+  </si>
+  <si>
+    <t>8*nestedExpr</t>
+  </si>
+  <si>
+    <t>4*nestedExpr</t>
+  </si>
+  <si>
+    <t>2*nextedExpr</t>
+  </si>
+  <si>
+    <t>1*nestedExpr</t>
+  </si>
+  <si>
+    <t>1*write</t>
+  </si>
+  <si>
+    <t>&lt;- 4 node'y posiadające pod soba 3 node'y: dwa nestedExpr o głębokości 2 i jeden '+'</t>
+  </si>
+  <si>
+    <t>&lt;- 8 node'ów posiadających pod sobą 3 node'y: dwie '1' i jeden '+'</t>
+  </si>
+  <si>
+    <t>Mutate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,8 +256,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -261,6 +280,2210 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>98535</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>164224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1497724</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>118241</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41169433-83AD-EDF4-34AE-9221E56831D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="98535" y="3212224"/>
+          <a:ext cx="6417879" cy="4145017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>grammar Sharp</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>program</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>action</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>)* | </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>EOF </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>action</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>assignment </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ifStatement </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>loop </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>write </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>);</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>scope</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'{' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>action</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>)* </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'}' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>loop</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'loop' constant scope </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>// loop 10 { }</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>read</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'read()'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>write</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'write' '(' expression ')' ';'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ifStatement</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'if (' condition ')' scope </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>// if (thing comp thing) { } ;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>condition</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>expression comparator expression </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>// thing comp thing //this must be evalueable to boolean</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>assignment</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>variable '=' expression ';' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>// x_1 = (2+(3*4))</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>expression</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>constant </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>variable </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>nestedExp </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>read </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>// this must evaluate to value</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>nestedExp</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'(' expression operator expression ')' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>// this also must evaluate to value</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="pl-PL" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>variable </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>VAR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>constant </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>operator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'*' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'/' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'+' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'-'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>comparator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'==' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'!=' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'&gt;' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'&lt;' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'&gt;=' </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>| </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'&lt;='</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: [0-9]+;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: [ \t\r\n]+ -&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>skip</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>VAR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>'x_'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>[0-9][0-9]*;   </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="pl-PL">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="pl-PL" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="pole tekstowe 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E37A39B-4A5A-D31B-357F-55E699C0B73F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8058150" y="1057275"/>
+          <a:ext cx="5476875" cy="1209675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Program składa się z jednej linijki: 'write', zawierającej w sobie </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>zrównoważone </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>drzewo sumujące 16 jedynek</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Załóżmy że chcemy to drzewo zcross'ować</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Jako punkt krosowania został wybrany expression o głębokości 5</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Z obliczeń usuwamy node program, bo nie chcemy krzyzować z rootem</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Na tych założeniach zbudowałem 2 pierwsze wiersze tego arkusza</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="pole tekstowe 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0198B0-3591-D418-F5B9-32F0636C2E77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7200900" y="2971800"/>
+          <a:ext cx="6105525" cy="1504950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Musiałem zmodyfikować wzór z prezentacji, ponieważ prawdopodobieństwa nie sumowały się do 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Prawdopodobieństwo na wybór gałęzi o tej samej wielkości było ok</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Jednak wzór przedstawiony jako prawdopodobieństwo wyboru podrzewa o innej głębokości, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>to tak naprawdę prawdopodobieństwo na wybór kontretnego poddrzewa spośród tych o innej</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> głębokości.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Problemem</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> jest współczynnik stojący w równaniu z prezentacji czynnik n+ stojący zaraz za znakiem dzielenia.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100"/>
+            <a:t>Aktualnie w komórce L2 jest on pominięty,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pl-PL" sz="1100" baseline="0"/>
+            <a:t> a w L3 jest wpisany zgodnie z formułą na prezentacji (odwróciłem znak podstawiając n- czyli C2, ponieważ liczone jest p- a nie p+)</a:t>
+          </a:r>
+          <a:endParaRPr lang="pl-PL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>379714</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>486359</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obraz 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE934A6A-AA9C-F019-9B88-329EE98BC8F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="379714" y="3171824"/>
+          <a:ext cx="4488145" cy="3371851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,7 +2786,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,218 +2809,218 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
+      <c r="A2" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="str">
         <f>"+Action"</f>
         <v>+Action</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="3"/>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="3"/>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="3"/>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="3"/>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="str">
         <f>"+Action"</f>
         <v>+Action</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -807,55 +3030,60 @@
     <mergeCell ref="A2:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C8AD3F-DE3B-4B12-A72F-BB3AA078B976}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="7" width="20" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>47</v>
-      </c>
-      <c r="M1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -892,11 +3120,11 @@
         <f>1-I2</f>
         <v>0.8</v>
       </c>
-      <c r="K2">
-        <f>J2/(B2*F2)</f>
+      <c r="K2" s="2">
+        <f>J2/F2</f>
         <v>0.15905044510385757</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <f>J2/G2</f>
         <v>0.64094955489614247</v>
       </c>
@@ -905,47 +3133,90 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L3" s="2">
+        <f>J2/(C2*G2)</f>
+        <v>1.4243323442136498E-2</v>
+      </c>
+    </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>51</v>
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>52</v>
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>53</v>
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>54</v>
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>55</v>
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>56</v>
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>